<commit_message>
Add composite state functionality
</commit_message>
<xml_diff>
--- a/Testing Sheet.xlsx
+++ b/Testing Sheet.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\University Work\Games Design - Year 3\AI - DAC619\Artificial_Intelligence_for_Games_(DAC619)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{2A312B72-3506-4F8B-BF65-966FAE23B5E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006FB16F-7860-46A4-8BCA-A342AB6E6110}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Fails as all AI never find health kit in scene. (Fixed, enter method was never called due to incorrect usage of state machine.)</t>
   </si>
@@ -61,12 +61,21 @@
   </si>
   <si>
     <t>Failed due to evaluating and constantly changing state back to the same one every tick update. (Fixed by making check if it was already in the selected state.)</t>
+  </si>
+  <si>
+    <t>State Comparison</t>
+  </si>
+  <si>
+    <t>Fails as GetType () returns the super class of the type given meaning that every state is the same as each other as they all implent interface IState&lt;T&gt;. (fixed)</t>
+  </si>
+  <si>
+    <t>Failed as it never bothered to pick up the health kit. (fixed as I needed to check if the item was in the inventory to keep the loop running with the new system in place.)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,11 +423,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -482,14 +491,22 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="2:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">

</xml_diff>